<commit_message>
Add Pretty Heroine and Magical Something
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="12045" windowHeight="5970" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="12045" windowHeight="5970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VP16-JP" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="26">
   <si>
     <t>:</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Booster SP: Destiny Soldiers</t>
+  </si>
+  <si>
+    <t>Magical Something</t>
+  </si>
+  <si>
+    <t>Abyss Actor - Pretty Heroine</t>
   </si>
 </sst>
 </file>
@@ -162,10 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,10 +559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -575,8 +582,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B2">
-        <v>100909081</v>
+        <v>100909000</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -587,7 +597,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>100909082</v>
+        <v>100909081</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -598,21 +608,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4">
+        <v>100909082</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5">
         <v>100909083</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>100909084</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -623,21 +630,24 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>100909084</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>100909085</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7">
-        <v>100909086</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -648,7 +658,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>100909087</v>
+        <v>100909086</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -659,7 +669,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>100909088</v>
+        <v>100909087</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -670,17 +680,29 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10">
+        <v>100909088</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11">
         <v>100909089</v>
       </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -688,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -956,6 +978,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
       <c r="B22">
         <v>100405021</v>
       </c>

</xml_diff>

<commit_message>
Add Abyss Actor - Extra
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
   <si>
     <t>:</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Abyss Actor - Pretty Heroine</t>
+  </si>
+  <si>
+    <t>Abyss Actor - Extra</t>
+  </si>
+  <si>
+    <t>Casting out the Darklords</t>
+  </si>
+  <si>
+    <t>Darklords Falling from Grace</t>
+  </si>
+  <si>
+    <t>Abyss Actor - Wild Hope</t>
+  </si>
+  <si>
+    <t>Abyss Script - Fantasy Magic</t>
+  </si>
+  <si>
+    <t>Abyss Script - Rise of the Dark Ruler</t>
   </si>
 </sst>
 </file>
@@ -708,15 +726,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.4609375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
@@ -967,6 +985,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
       <c r="B21">
         <v>100405020</v>
       </c>
@@ -992,6 +1013,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
       <c r="B23">
         <v>100405022</v>
       </c>
@@ -1003,6 +1027,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
       <c r="B24">
         <v>100405023</v>
       </c>
@@ -1050,6 +1077,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
       <c r="B28">
         <v>100405027</v>
       </c>
@@ -1110,6 +1140,67 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>100405032</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>100405033</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>100405034</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>100405035</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>100405036</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ancient Gear and Darklord update
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -10,13 +10,14 @@
     <sheet name="VP16-JP" sheetId="2" r:id="rId1"/>
     <sheet name="TDIL-EN" sheetId="4" r:id="rId2"/>
     <sheet name="SPDS-JP" sheetId="5" r:id="rId3"/>
+    <sheet name="SR03-JP" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
   <si>
     <t>:</t>
   </si>
@@ -112,6 +113,21 @@
   </si>
   <si>
     <t>Abyss Script - Rise of the Dark Ruler</t>
+  </si>
+  <si>
+    <t>Structure Deck R: Machine Dragon Re-Volt</t>
+  </si>
+  <si>
+    <t>Ancient Gear Gadget</t>
+  </si>
+  <si>
+    <t>Ancient Gear Reactor Dragon</t>
+  </si>
+  <si>
+    <t>Ancient Gear Catapult</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
@@ -186,11 +202,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +512,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -580,7 +597,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -729,7 +746,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1208,4 +1225,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4">
+        <v>42637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>100303000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>100303001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>100303021</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add D3 and new Abyss Scripts
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
   <si>
     <t>:</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>D3</t>
   </si>
 </sst>
 </file>
@@ -745,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -847,6 +850,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
       <c r="B8">
         <v>100405007</v>
       </c>

</xml_diff>

<commit_message>
Almost forgot to add Ancient Gear Token
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="39">
   <si>
     <t>:</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>D3</t>
+  </si>
+  <si>
+    <t>Ancient Gear Token</t>
   </si>
 </sst>
 </file>
@@ -748,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1235,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1299,6 +1302,20 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>100303121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Darklords to excel sheet
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="42">
   <si>
     <t>:</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Ancient Gear Token</t>
+  </si>
+  <si>
+    <t>Darklord Mastema</t>
+  </si>
+  <si>
+    <t>Altar of the Darklords</t>
+  </si>
+  <si>
+    <t>Darklords' Temptation</t>
   </si>
 </sst>
 </file>
@@ -749,10 +758,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1170,6 +1179,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
       <c r="B33">
         <v>100405032</v>
       </c>
@@ -1206,6 +1218,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
       <c r="B36">
         <v>100405035</v>
       </c>
@@ -1227,6 +1242,53 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>100405037</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>100405038</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>100405039</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>100405040</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update database for MVP1-EN and TDIL-EN
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="12045" windowHeight="5970" activeTab="2"/>
+    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VP16-JP" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="53">
   <si>
     <t>:</t>
   </si>
@@ -143,6 +143,39 @@
   </si>
   <si>
     <t>Darklords' Temptation</t>
+  </si>
+  <si>
+    <t>Ninjitsu Art Notebook</t>
+  </si>
+  <si>
+    <t>Subterror Nemesis Warrior</t>
+  </si>
+  <si>
+    <t>Subterror Behemoth Umastryx</t>
+  </si>
+  <si>
+    <t>SPYRAL Super Agent</t>
+  </si>
+  <si>
+    <t>SPYRAL Quik-Fix</t>
+  </si>
+  <si>
+    <t>SPYRAL GEAR - Drone</t>
+  </si>
+  <si>
+    <t>SPYRAL GEAR - Big Red</t>
+  </si>
+  <si>
+    <t>Abyss Actor - Sassy Rookie</t>
+  </si>
+  <si>
+    <t>Abyss Script - Abode of the Fire Dragon</t>
+  </si>
+  <si>
+    <t>Abyss Stage Prop - Escape Stage Coach</t>
+  </si>
+  <si>
+    <t>Entering the Abyss Actor Dressing Room</t>
   </si>
 </sst>
 </file>
@@ -612,7 +645,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -646,6 +679,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
       <c r="B3">
         <v>100909081</v>
       </c>
@@ -657,6 +693,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
       <c r="B4">
         <v>100909082</v>
       </c>
@@ -668,6 +707,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
       <c r="B5">
         <v>100909083</v>
       </c>
@@ -707,6 +749,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
       <c r="B8">
         <v>100909086</v>
       </c>
@@ -718,6 +763,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
       <c r="B9">
         <v>100909087</v>
       </c>
@@ -729,6 +777,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
       <c r="B10">
         <v>100909088</v>
       </c>
@@ -740,6 +791,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
       <c r="B11">
         <v>100909089</v>
       </c>
@@ -758,15 +812,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.23046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
@@ -891,7 +945,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>100405009</v>
+        <v>100405010</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -902,7 +956,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>100405010</v>
+        <v>100405011</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -913,7 +967,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>100405011</v>
+        <v>100405013</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -924,7 +978,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>100405012</v>
+        <v>100405015</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -934,8 +988,11 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
       <c r="B14">
-        <v>100405013</v>
+        <v>100405016</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -945,8 +1002,11 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
       <c r="B15">
-        <v>100405014</v>
+        <v>100405017</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -956,8 +1016,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
       <c r="B16">
-        <v>100405015</v>
+        <v>100405018</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -968,10 +1031,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B17">
-        <v>100405016</v>
+        <v>100405019</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -982,10 +1045,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B18">
-        <v>100405017</v>
+        <v>100405020</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
@@ -996,10 +1059,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>100405018</v>
+        <v>100405021</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -1009,8 +1072,11 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
       <c r="B20">
-        <v>100405019</v>
+        <v>100405022</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -1021,10 +1087,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B21">
-        <v>100405020</v>
+        <v>100405023</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -1035,10 +1101,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B22">
-        <v>100405021</v>
+        <v>100405024</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -1049,10 +1115,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B23">
-        <v>100405022</v>
+        <v>100405025</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -1063,10 +1129,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B24">
-        <v>100405023</v>
+        <v>100405026</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
@@ -1077,10 +1143,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B25">
-        <v>100405024</v>
+        <v>100405027</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -1090,8 +1156,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
       <c r="B26">
-        <v>100405025</v>
+        <v>100405028</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
@@ -1101,8 +1170,11 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
       <c r="B27">
-        <v>100405026</v>
+        <v>100405029</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
@@ -1113,10 +1185,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B28">
-        <v>100405027</v>
+        <v>100405030</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
@@ -1126,8 +1198,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
       <c r="B29">
-        <v>100405028</v>
+        <v>100405031</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
@@ -1138,10 +1213,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B30">
-        <v>100405029</v>
+        <v>100405032</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -1151,11 +1226,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>15</v>
-      </c>
       <c r="B31">
-        <v>100405030</v>
+        <v>100405033</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
@@ -1166,10 +1238,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B32">
-        <v>100405031</v>
+        <v>100405034</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
@@ -1180,10 +1252,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B33">
-        <v>100405032</v>
+        <v>100405035</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -1193,8 +1265,11 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
       <c r="B34">
-        <v>100405033</v>
+        <v>100405036</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -1205,10 +1280,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B35">
-        <v>100405034</v>
+        <v>100405037</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
@@ -1218,11 +1293,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
       <c r="B36">
-        <v>100405035</v>
+        <v>100405038</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
@@ -1232,11 +1304,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>28</v>
-      </c>
       <c r="B37">
-        <v>100405036</v>
+        <v>100405039</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
@@ -1246,49 +1315,13 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>41</v>
-      </c>
       <c r="B38">
-        <v>100405037</v>
+        <v>100405040</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B39">
-        <v>100405038</v>
-      </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B40">
-        <v>100405039</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B41">
-        <v>100405040</v>
-      </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update IDs and Abyss Actor setcodes
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970" activeTab="2"/>
+    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970"/>
   </bookViews>
   <sheets>
-    <sheet name="VP16-JP" sheetId="2" r:id="rId1"/>
-    <sheet name="TDIL-EN" sheetId="4" r:id="rId2"/>
-    <sheet name="SPDS-JP" sheetId="5" r:id="rId3"/>
-    <sheet name="SR03-JP" sheetId="6" r:id="rId4"/>
+    <sheet name="TDIL-EN" sheetId="4" r:id="rId1"/>
+    <sheet name="SPDS-JP" sheetId="5" r:id="rId2"/>
+    <sheet name="SR03-JP" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
   <si>
     <t>:</t>
   </si>
@@ -71,21 +70,6 @@
   </si>
   <si>
     <t>The Dark Illusion (TCG)</t>
-  </si>
-  <si>
-    <t>20th Rival Collection</t>
-  </si>
-  <si>
-    <t>Destiny HERO - Deadlyguy</t>
-  </si>
-  <si>
-    <t>Red Rising Dragon</t>
-  </si>
-  <si>
-    <t>Galaxy-Eyes Cipher Blade Dragon</t>
-  </si>
-  <si>
-    <t>Abyss Actor - Dandy Supporting Actor</t>
   </si>
   <si>
     <t>Booster SP: Destiny Soldiers</t>
@@ -557,94 +541,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2">
-        <v>42572</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>100208001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>100208002</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>100208003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>100208004</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -666,7 +565,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>100909000</v>
@@ -680,7 +579,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>100909081</v>
@@ -694,7 +593,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>100909082</v>
@@ -708,7 +607,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>100909083</v>
@@ -750,7 +649,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>100909086</v>
@@ -764,7 +663,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>100909087</v>
@@ -778,7 +677,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>100909088</v>
@@ -792,7 +691,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>100909089</v>
@@ -810,11 +709,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +727,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2">
         <v>42588</v>
@@ -917,7 +816,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>100405007</v>
@@ -1031,7 +930,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>100405019</v>
@@ -1045,7 +944,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>100405020</v>
@@ -1059,7 +958,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>100405021</v>
@@ -1073,7 +972,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>100405022</v>
@@ -1087,7 +986,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>100405023</v>
@@ -1115,7 +1014,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>100405025</v>
@@ -1129,7 +1028,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <v>100405026</v>
@@ -1143,7 +1042,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>100405027</v>
@@ -1157,7 +1056,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B26">
         <v>100405028</v>
@@ -1213,7 +1112,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>100405032</v>
@@ -1238,7 +1137,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>100405034</v>
@@ -1252,7 +1151,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>100405035</v>
@@ -1266,7 +1165,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B34">
         <v>100405036</v>
@@ -1280,7 +1179,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>100405037</v>
@@ -1331,7 +1230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1349,7 +1248,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4">
         <v>42637</v>
@@ -1357,7 +1256,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>100303000</v>
@@ -1366,12 +1265,12 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>100303001</v>
@@ -1380,12 +1279,12 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>100303021</v>
@@ -1394,12 +1293,12 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>100303121</v>
@@ -1408,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add D-HERO Celestial to ID sheet
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970"/>
+    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TDIL-EN" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
   <si>
     <t>:</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Entering the Abyss Actor Dressing Room</t>
+  </si>
+  <si>
+    <t>Destiny HERO - Celestial</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -713,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -804,6 +807,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
       <c r="B7">
         <v>100405006</v>
       </c>

</xml_diff>

<commit_message>
Add Metal Claw and Darklord Amdusias
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="50">
   <si>
     <t>:</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Destiny HERO - Celestial</t>
+  </si>
+  <si>
+    <t>Darklord Amdusias</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1131,6 +1134,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
       <c r="B31">
         <v>100405033</v>
       </c>

</xml_diff>

<commit_message>
Add new RATE cards and update ID for Delta the Magnet Warrior
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="118">
   <si>
     <t>:</t>
   </si>
@@ -365,6 +365,15 @@
   </si>
   <si>
     <t>Rank-Up-Magic Cipher Ascension</t>
+  </si>
+  <si>
+    <t>Speedroid Bamboo Horse</t>
+  </si>
+  <si>
+    <t>Wind Witch - Ice Bell</t>
+  </si>
+  <si>
+    <t>Cipher Spectrum</t>
   </si>
 </sst>
 </file>
@@ -2018,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -2056,6 +2065,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>100911002</v>
+      </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -2064,6 +2076,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>100911003</v>
+      </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -2072,6 +2087,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>100911004</v>
+      </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -2083,6 +2101,9 @@
       <c r="A6" t="s">
         <v>108</v>
       </c>
+      <c r="B6">
+        <v>100911005</v>
+      </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -2091,6 +2112,12 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7">
+        <v>100911006</v>
+      </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -2099,6 +2126,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8">
+        <v>100911007</v>
+      </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
@@ -2121,6 +2154,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>100911009</v>
+      </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
@@ -2129,6 +2165,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>100911010</v>
+      </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -2140,6 +2179,9 @@
       <c r="A12" t="s">
         <v>110</v>
       </c>
+      <c r="B12">
+        <v>100911011</v>
+      </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -2148,6 +2190,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>100911012</v>
+      </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
@@ -2156,6 +2201,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>100911013</v>
+      </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
@@ -2164,6 +2212,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>100911014</v>
+      </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
@@ -2172,6 +2223,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>100911015</v>
+      </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
@@ -2179,7 +2233,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>100911016</v>
+      </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
@@ -2187,7 +2244,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>100911017</v>
+      </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2255,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>100911018</v>
+      </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
@@ -2203,7 +2266,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>100911019</v>
+      </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
@@ -2211,7 +2277,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>100911020</v>
+      </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
@@ -2219,7 +2288,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>100911021</v>
+      </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2299,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>100911022</v>
+      </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2310,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>100911023</v>
+      </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
@@ -2243,7 +2321,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>100911024</v>
+      </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2332,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>100911025</v>
+      </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
@@ -2259,7 +2343,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>100911026</v>
+      </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
@@ -2267,7 +2354,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>100911027</v>
+      </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
@@ -2275,7 +2365,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>100911028</v>
+      </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
@@ -2283,7 +2376,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>100911029</v>
+      </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
@@ -2291,7 +2387,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>100911030</v>
+      </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
@@ -2299,7 +2398,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>100911031</v>
+      </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
@@ -2308,6 +2410,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>100911032</v>
+      </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
@@ -2316,6 +2421,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>100911033</v>
+      </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
@@ -2324,6 +2432,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>100911034</v>
+      </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
@@ -2332,6 +2443,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>100911035</v>
+      </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
@@ -2340,6 +2454,9 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>100911036</v>
+      </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
@@ -2348,6 +2465,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>100911037</v>
+      </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
@@ -2356,6 +2476,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>100911038</v>
+      </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
@@ -2378,6 +2501,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>100911040</v>
+      </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
@@ -2386,6 +2512,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>100911041</v>
+      </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
@@ -2394,6 +2523,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>100911042</v>
+      </c>
       <c r="C43" t="s">
         <v>0</v>
       </c>
@@ -2416,6 +2548,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>100911044</v>
+      </c>
       <c r="C45" t="s">
         <v>0</v>
       </c>
@@ -2424,6 +2559,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>100911045</v>
+      </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
@@ -2432,6 +2570,9 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>100911046</v>
+      </c>
       <c r="C47" t="s">
         <v>0</v>
       </c>
@@ -2440,6 +2581,9 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>100911047</v>
+      </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
@@ -2448,6 +2592,9 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>100911048</v>
+      </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
@@ -2459,6 +2606,9 @@
       <c r="A50" t="s">
         <v>113</v>
       </c>
+      <c r="B50">
+        <v>100911049</v>
+      </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
@@ -2467,6 +2617,9 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>100911050</v>
+      </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
@@ -2475,6 +2628,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>100911051</v>
+      </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
@@ -2483,6 +2639,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>100911052</v>
+      </c>
       <c r="C53" t="s">
         <v>0</v>
       </c>
@@ -2491,6 +2650,9 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>100911053</v>
+      </c>
       <c r="C54" t="s">
         <v>0</v>
       </c>
@@ -2499,6 +2661,9 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>100911054</v>
+      </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
@@ -2507,6 +2672,9 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>100911055</v>
+      </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
@@ -2518,6 +2686,9 @@
       <c r="A57" t="s">
         <v>114</v>
       </c>
+      <c r="B57">
+        <v>100911056</v>
+      </c>
       <c r="C57" t="s">
         <v>0</v>
       </c>
@@ -2526,6 +2697,9 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>100911057</v>
+      </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
@@ -2534,6 +2708,9 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>100911058</v>
+      </c>
       <c r="C59" t="s">
         <v>0</v>
       </c>
@@ -2542,6 +2719,9 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>100911059</v>
+      </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
@@ -2550,6 +2730,9 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>100911060</v>
+      </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
@@ -2558,6 +2741,9 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>100911061</v>
+      </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
@@ -2566,6 +2752,9 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>100911062</v>
+      </c>
       <c r="C63" t="s">
         <v>0</v>
       </c>
@@ -2574,6 +2763,9 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>100911063</v>
+      </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2773,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>100911064</v>
+      </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
@@ -2589,7 +2784,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>100911065</v>
+      </c>
       <c r="C66" t="s">
         <v>0</v>
       </c>
@@ -2597,7 +2795,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>100911066</v>
+      </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2806,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>100911067</v>
+      </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
@@ -2613,7 +2817,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>100911068</v>
+      </c>
       <c r="C69" t="s">
         <v>0</v>
       </c>
@@ -2621,7 +2828,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70">
+        <v>100911069</v>
+      </c>
       <c r="C70" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +2842,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>100911070</v>
+      </c>
       <c r="C71" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2853,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>100911071</v>
+      </c>
       <c r="C72" t="s">
         <v>0</v>
       </c>
@@ -2645,7 +2864,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>100911072</v>
+      </c>
       <c r="C73" t="s">
         <v>0</v>
       </c>
@@ -2653,7 +2875,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>100911073</v>
+      </c>
       <c r="C74" t="s">
         <v>0</v>
       </c>
@@ -2661,7 +2886,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>100911074</v>
+      </c>
       <c r="C75" t="s">
         <v>0</v>
       </c>
@@ -2669,7 +2897,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>100911075</v>
+      </c>
       <c r="C76" t="s">
         <v>0</v>
       </c>
@@ -2677,7 +2908,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>100911076</v>
+      </c>
       <c r="C77" t="s">
         <v>0</v>
       </c>
@@ -2685,7 +2919,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>100911077</v>
+      </c>
       <c r="C78" t="s">
         <v>0</v>
       </c>
@@ -2693,7 +2930,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>100911078</v>
+      </c>
       <c r="C79" t="s">
         <v>0</v>
       </c>
@@ -2701,7 +2941,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>100911079</v>
+      </c>
       <c r="C80" t="s">
         <v>0</v>
       </c>
@@ -2709,19 +2952,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>100911080</v>
+      </c>
       <c r="C81" t="s">
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C82" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New cards and update ID sheet
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970" activeTab="6"/>
+    <workbookView xWindow="3945" yWindow="1260" windowWidth="12045" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="LDK2-EN" sheetId="10" r:id="rId1"/>
-    <sheet name="SDMY-EN" sheetId="13" r:id="rId2"/>
-    <sheet name="SDKS-EN" sheetId="14" r:id="rId3"/>
-    <sheet name="INOV-EN" sheetId="15" r:id="rId4"/>
-    <sheet name="SPDS-EN" sheetId="5" r:id="rId5"/>
-    <sheet name="SDPD-EN" sheetId="16" r:id="rId6"/>
-    <sheet name="RATE-JP" sheetId="11" r:id="rId7"/>
+    <sheet name="RATE-JP" sheetId="11" r:id="rId2"/>
+    <sheet name="SDMY-EN" sheetId="13" r:id="rId3"/>
+    <sheet name="SDKS-EN" sheetId="14" r:id="rId4"/>
+    <sheet name="INOV-EN" sheetId="15" r:id="rId5"/>
+    <sheet name="SPFE-JP" sheetId="17" r:id="rId6"/>
+    <sheet name="SPDS-EN" sheetId="5" r:id="rId7"/>
+    <sheet name="SDPD-EN" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="249">
   <si>
     <t>:</t>
   </si>
@@ -650,6 +651,123 @@
   </si>
   <si>
     <t>Juunishishi no Hougou</t>
+  </si>
+  <si>
+    <t>Performapal Dag Daggerman</t>
+  </si>
+  <si>
+    <t>Performapal Laughmaker</t>
+  </si>
+  <si>
+    <t>Parasite Fusioner</t>
+  </si>
+  <si>
+    <t>Flower Cardian Cherry Blossom with Curtain</t>
+  </si>
+  <si>
+    <t>True King Lithosazim, the Disaster</t>
+  </si>
+  <si>
+    <t>Esprit Bird - Shinobi Garasu</t>
+  </si>
+  <si>
+    <t>Esprit Bird - Den Hato</t>
+  </si>
+  <si>
+    <t>Envoy of Chaos</t>
+  </si>
+  <si>
+    <t>Tierra, Goddess of Rebirth</t>
+  </si>
+  <si>
+    <t>Apprentice Piper</t>
+  </si>
+  <si>
+    <t>All-Consuming Glutton</t>
+  </si>
+  <si>
+    <t>Wightprincess</t>
+  </si>
+  <si>
+    <t>Metrognome</t>
+  </si>
+  <si>
+    <t>Fairy Tail - Cinderella</t>
+  </si>
+  <si>
+    <t>Wind Witch - Crystal Bell</t>
+  </si>
+  <si>
+    <t>Flower Cardian Five Lights</t>
+  </si>
+  <si>
+    <t>Crystron Glyongandr</t>
+  </si>
+  <si>
+    <t>Homuragami - Shiranui</t>
+  </si>
+  <si>
+    <t>Heavy-Armored Train Iron Wolf‎‎</t>
+  </si>
+  <si>
+    <t>Card Regeneration</t>
+  </si>
+  <si>
+    <t>Super Soldier Origin</t>
+  </si>
+  <si>
+    <t>Ritual Beast's Return</t>
+  </si>
+  <si>
+    <t>Lawnmowing Next Door</t>
+  </si>
+  <si>
+    <t>Terminal World Next</t>
+  </si>
+  <si>
+    <t>Bewildering Wind</t>
+  </si>
+  <si>
+    <t>Universal Beginning</t>
+  </si>
+  <si>
+    <t>Majespecter Gust</t>
+  </si>
+  <si>
+    <t>Void Madness</t>
+  </si>
+  <si>
+    <t>Switch Hero</t>
+  </si>
+  <si>
+    <t>Booster SP: Fusion Enforcers</t>
+  </si>
+  <si>
+    <t>Predator Plant Sundew Kingii</t>
+  </si>
+  <si>
+    <t>Predator Plant Chimera Rafflesia</t>
+  </si>
+  <si>
+    <t>Greedy Venom Fusion Dragon</t>
+  </si>
+  <si>
+    <t>Predator Planter</t>
+  </si>
+  <si>
+    <t>Frightfur Kraken</t>
+  </si>
+  <si>
+    <t>Aleister the Eidolon Summoner</t>
+  </si>
+  <si>
+    <t>Raideen the Eidolon Beast</t>
+  </si>
+  <si>
+    <t>Elysion the Eidolon Beast</t>
+  </si>
+  <si>
+    <t>Eidolon Summoning Magic</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1119,10 +1239,1187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.4609375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2">
+        <v>42651</v>
+      </c>
+      <c r="F1" s="10">
+        <v>42424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>100911001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3">
+        <v>100911002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4">
+        <v>100911003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5">
+        <v>100911004</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>100911005</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>100911006</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>100911007</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>100911008</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10">
+        <v>100911009</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11">
+        <v>100911010</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>100911011</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13">
+        <v>100911012</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14">
+        <v>100911013</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15">
+        <v>100911014</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16">
+        <v>100911015</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <v>100911016</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18">
+        <v>100911017</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19">
+        <v>100911018</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20">
+        <v>100911019</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21">
+        <v>100911020</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22">
+        <v>100911021</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23">
+        <v>100911022</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24">
+        <v>100911023</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25">
+        <v>100911024</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26">
+        <v>100911025</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27">
+        <v>100911026</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28">
+        <v>100911027</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29">
+        <v>100911028</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30">
+        <v>100911029</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31">
+        <v>100911030</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32">
+        <v>100911031</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33">
+        <v>100911032</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34">
+        <v>100911033</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35">
+        <v>100911034</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36">
+        <v>100911035</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37">
+        <v>100911036</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38">
+        <v>100911037</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39">
+        <v>100911038</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>100911039</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41">
+        <v>100911040</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42">
+        <v>100911041</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43">
+        <v>100911042</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>100911043</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45">
+        <v>100911044</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B46">
+        <v>100911045</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B47">
+        <v>100911046</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>227</v>
+      </c>
+      <c r="B48">
+        <v>100911047</v>
+      </c>
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49">
+        <v>100911048</v>
+      </c>
+      <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>100911049</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51">
+        <v>100911050</v>
+      </c>
+      <c r="C51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>193</v>
+      </c>
+      <c r="B52">
+        <v>100911051</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53">
+        <v>100911052</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54">
+        <v>100911053</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55">
+        <v>100911054</v>
+      </c>
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56">
+        <v>100911055</v>
+      </c>
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57">
+        <v>100911056</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58">
+        <v>100911057</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>208</v>
+      </c>
+      <c r="B59">
+        <v>100911058</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60">
+        <v>100911059</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61">
+        <v>100911060</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>200</v>
+      </c>
+      <c r="B62">
+        <v>100911061</v>
+      </c>
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63">
+        <v>100911062</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>201</v>
+      </c>
+      <c r="B64">
+        <v>100911063</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>231</v>
+      </c>
+      <c r="B65">
+        <v>100911064</v>
+      </c>
+      <c r="C65" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>202</v>
+      </c>
+      <c r="B66">
+        <v>100911065</v>
+      </c>
+      <c r="C66" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>232</v>
+      </c>
+      <c r="B67">
+        <v>100911066</v>
+      </c>
+      <c r="C67" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>233</v>
+      </c>
+      <c r="B68">
+        <v>100911067</v>
+      </c>
+      <c r="C68" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>234</v>
+      </c>
+      <c r="B69">
+        <v>100911068</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70">
+        <v>100911069</v>
+      </c>
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71">
+        <v>100911070</v>
+      </c>
+      <c r="C71" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72">
+        <v>100911071</v>
+      </c>
+      <c r="C72" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>204</v>
+      </c>
+      <c r="B73">
+        <v>100911072</v>
+      </c>
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74">
+        <v>100911073</v>
+      </c>
+      <c r="C74" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75">
+        <v>100911074</v>
+      </c>
+      <c r="C75" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>236</v>
+      </c>
+      <c r="B76">
+        <v>100911075</v>
+      </c>
+      <c r="C76" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>237</v>
+      </c>
+      <c r="B77">
+        <v>100911076</v>
+      </c>
+      <c r="C77" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78">
+        <v>100911077</v>
+      </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>207</v>
+      </c>
+      <c r="B79">
+        <v>100911078</v>
+      </c>
+      <c r="C79" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>238</v>
+      </c>
+      <c r="B80">
+        <v>100911079</v>
+      </c>
+      <c r="C80" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>100911080</v>
+      </c>
+      <c r="C81" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>208</v>
+      </c>
+      <c r="B82">
+        <v>100911100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>209</v>
+      </c>
+      <c r="B83">
+        <v>100911102</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" r:id="rId1" tooltip="Ancient Gear Hunting Hound" display="http://yugioh.wikia.com/wiki/Ancient_Gear_Hunting_Hound"/>
+    <hyperlink ref="A15" r:id="rId2" tooltip="Juunishishi Molmorat" display="http://yugioh.wikia.com/wiki/Juunishishi_Molmorat"/>
+    <hyperlink ref="A16" r:id="rId3" tooltip="Juunishishi Rabbina" display="http://yugioh.wikia.com/wiki/Juunishishi_Rabbina"/>
+    <hyperlink ref="A17" r:id="rId4" tooltip="Juunishishi Viper" display="http://yugioh.wikia.com/wiki/Juunishishi_Viper"/>
+    <hyperlink ref="A18" r:id="rId5" tooltip="Juunishishi Thoroughblade" display="http://yugioh.wikia.com/wiki/Juunishishi_Thoroughblade"/>
+    <hyperlink ref="A19" r:id="rId6" tooltip="Juunishishi Ram" display="http://yugioh.wikia.com/wiki/Juunishishi_Ram"/>
+    <hyperlink ref="A21" r:id="rId7" tooltip="Crystron Rion" display="http://yugioh.wikia.com/wiki/Crystron_Rion"/>
+    <hyperlink ref="A22" r:id="rId8" tooltip="Crystron Sulphafnir" display="http://yugioh.wikia.com/wiki/Crystron_Sulphafnir"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1196,7 +2493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1273,7 +2570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B81"/>
   <sheetViews>
@@ -1700,12 +2997,530 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="1.3828125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="6">
+        <v>42686</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>100406001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>100406002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>100406003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>100406004</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6">
+        <v>100406005</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>100406006</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>100406007</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>100406008</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10">
+        <v>100406009</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11">
+        <v>100406010</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12">
+        <v>100406011</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>100406012</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>100406013</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>100406015</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>100406016</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>100406017</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>100406019</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19">
+        <v>100406020</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>100406021</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>100406022</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>100406023</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>100406024</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24">
+        <v>100406026</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>100406027</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26">
+        <v>100406028</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>100406029</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>100406030</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>100406031</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>100406032</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31">
+        <v>100406033</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>100406034</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B33">
+        <v>100406035</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>100406036</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>100406037</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>100406038</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>100406039</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>100406040</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>100406041</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>100406042</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>100406043</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>100406044</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>100406045</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1974,7 +3789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -2074,1088 +3889,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="33.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.61328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.4609375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="2">
-        <v>42651</v>
-      </c>
-      <c r="F1" s="10">
-        <v>42424</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2">
-        <v>100911001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3">
-        <v>100911002</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4">
-        <v>100911003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <v>100911004</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6">
-        <v>100911005</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7">
-        <v>100911006</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8">
-        <v>100911007</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9">
-        <v>100911008</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>100911009</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B11">
-        <v>100911010</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>100911011</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13">
-        <v>100911012</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14">
-        <v>100911013</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15">
-        <v>100911014</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16">
-        <v>100911015</v>
-      </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17">
-        <v>100911016</v>
-      </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18">
-        <v>100911017</v>
-      </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19">
-        <v>100911018</v>
-      </c>
-      <c r="C19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20">
-        <v>100911019</v>
-      </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>179</v>
-      </c>
-      <c r="B21">
-        <v>100911020</v>
-      </c>
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B22">
-        <v>100911021</v>
-      </c>
-      <c r="C22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B23">
-        <v>100911022</v>
-      </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24">
-        <v>100911023</v>
-      </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B25">
-        <v>100911024</v>
-      </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B26">
-        <v>100911025</v>
-      </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27">
-        <v>100911026</v>
-      </c>
-      <c r="C27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28">
-        <v>100911027</v>
-      </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B29">
-        <v>100911028</v>
-      </c>
-      <c r="C29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B30">
-        <v>100911029</v>
-      </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>184</v>
-      </c>
-      <c r="B31">
-        <v>100911030</v>
-      </c>
-      <c r="C31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32">
-        <v>100911031</v>
-      </c>
-      <c r="C32" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B33">
-        <v>100911032</v>
-      </c>
-      <c r="C33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B34">
-        <v>100911033</v>
-      </c>
-      <c r="C34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B35">
-        <v>100911034</v>
-      </c>
-      <c r="C35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B36">
-        <v>100911035</v>
-      </c>
-      <c r="C36" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>186</v>
-      </c>
-      <c r="B37">
-        <v>100911036</v>
-      </c>
-      <c r="C37" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>187</v>
-      </c>
-      <c r="B38">
-        <v>100911037</v>
-      </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>188</v>
-      </c>
-      <c r="B39">
-        <v>100911038</v>
-      </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40">
-        <v>100911039</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B41">
-        <v>100911040</v>
-      </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>189</v>
-      </c>
-      <c r="B42">
-        <v>100911041</v>
-      </c>
-      <c r="C42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>190</v>
-      </c>
-      <c r="B43">
-        <v>100911042</v>
-      </c>
-      <c r="C43" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44">
-        <v>100911043</v>
-      </c>
-      <c r="C44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>191</v>
-      </c>
-      <c r="B45">
-        <v>100911044</v>
-      </c>
-      <c r="C45" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B46">
-        <v>100911045</v>
-      </c>
-      <c r="C46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B47">
-        <v>100911046</v>
-      </c>
-      <c r="C47" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B48">
-        <v>100911047</v>
-      </c>
-      <c r="C48" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>192</v>
-      </c>
-      <c r="B49">
-        <v>100911048</v>
-      </c>
-      <c r="C49" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50">
-        <v>100911049</v>
-      </c>
-      <c r="C50" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B51">
-        <v>100911050</v>
-      </c>
-      <c r="C51" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>193</v>
-      </c>
-      <c r="B52">
-        <v>100911051</v>
-      </c>
-      <c r="C52" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>194</v>
-      </c>
-      <c r="B53">
-        <v>100911052</v>
-      </c>
-      <c r="C53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>195</v>
-      </c>
-      <c r="B54">
-        <v>100911053</v>
-      </c>
-      <c r="C54" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>196</v>
-      </c>
-      <c r="B55">
-        <v>100911054</v>
-      </c>
-      <c r="C55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>197</v>
-      </c>
-      <c r="B56">
-        <v>100911055</v>
-      </c>
-      <c r="C56" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57">
-        <v>100911056</v>
-      </c>
-      <c r="C57" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B58">
-        <v>100911057</v>
-      </c>
-      <c r="C58" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B59">
-        <v>100911058</v>
-      </c>
-      <c r="C59" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>198</v>
-      </c>
-      <c r="B60">
-        <v>100911059</v>
-      </c>
-      <c r="C60" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>199</v>
-      </c>
-      <c r="B61">
-        <v>100911060</v>
-      </c>
-      <c r="C61" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>200</v>
-      </c>
-      <c r="B62">
-        <v>100911061</v>
-      </c>
-      <c r="C62" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B63">
-        <v>100911062</v>
-      </c>
-      <c r="C63" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>201</v>
-      </c>
-      <c r="B64">
-        <v>100911063</v>
-      </c>
-      <c r="C64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B65">
-        <v>100911064</v>
-      </c>
-      <c r="C65" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>202</v>
-      </c>
-      <c r="B66">
-        <v>100911065</v>
-      </c>
-      <c r="C66" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B67">
-        <v>100911066</v>
-      </c>
-      <c r="C67" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B68">
-        <v>100911067</v>
-      </c>
-      <c r="C68" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B69">
-        <v>100911068</v>
-      </c>
-      <c r="C69" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>51</v>
-      </c>
-      <c r="B70">
-        <v>100911069</v>
-      </c>
-      <c r="C70" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>203</v>
-      </c>
-      <c r="B71">
-        <v>100911070</v>
-      </c>
-      <c r="C71" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B72">
-        <v>100911071</v>
-      </c>
-      <c r="C72" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>204</v>
-      </c>
-      <c r="B73">
-        <v>100911072</v>
-      </c>
-      <c r="C73" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B74">
-        <v>100911073</v>
-      </c>
-      <c r="C74" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>205</v>
-      </c>
-      <c r="B75">
-        <v>100911074</v>
-      </c>
-      <c r="C75" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B76">
-        <v>100911075</v>
-      </c>
-      <c r="C76" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B77">
-        <v>100911076</v>
-      </c>
-      <c r="C77" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>206</v>
-      </c>
-      <c r="B78">
-        <v>100911077</v>
-      </c>
-      <c r="C78" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>207</v>
-      </c>
-      <c r="B79">
-        <v>100911078</v>
-      </c>
-      <c r="C79" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B80">
-        <v>100911079</v>
-      </c>
-      <c r="C80" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B81">
-        <v>100911080</v>
-      </c>
-      <c r="C81" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>208</v>
-      </c>
-      <c r="B82">
-        <v>100911100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>209</v>
-      </c>
-      <c r="B83">
-        <v>100911102</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1" tooltip="Ancient Gear Hunting Hound" display="http://yugioh.wikia.com/wiki/Ancient_Gear_Hunting_Hound"/>
-    <hyperlink ref="A15" r:id="rId2" tooltip="Juunishishi Molmorat" display="http://yugioh.wikia.com/wiki/Juunishishi_Molmorat"/>
-    <hyperlink ref="A16" r:id="rId3" tooltip="Juunishishi Rabbina" display="http://yugioh.wikia.com/wiki/Juunishishi_Rabbina"/>
-    <hyperlink ref="A17" r:id="rId4" tooltip="Juunishishi Viper" display="http://yugioh.wikia.com/wiki/Juunishishi_Viper"/>
-    <hyperlink ref="A18" r:id="rId5" tooltip="Juunishishi Thoroughblade" display="http://yugioh.wikia.com/wiki/Juunishishi_Thoroughblade"/>
-    <hyperlink ref="A19" r:id="rId6" tooltip="Juunishishi Ram" display="http://yugioh.wikia.com/wiki/Juunishishi_Ram"/>
-    <hyperlink ref="A21" r:id="rId7" tooltip="Crystron Rion" display="http://yugioh.wikia.com/wiki/Crystron_Rion"/>
-    <hyperlink ref="A22" r:id="rId8" tooltip="Crystron Sulphafnir" display="http://yugioh.wikia.com/wiki/Crystron_Sulphafnir"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Predaplant Sundew Kingii
If it's on FH, then it has to be passable
</commit_message>
<xml_diff>
--- a/documentation/ygopro id sheet.xlsx
+++ b/documentation/ygopro id sheet.xlsx
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="B2:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -924,18 +924,18 @@
     <col min="2" max="2" width="26.61328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.3828125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="1.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="3">
-        <v>42686</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -951,8 +951,11 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>100406001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -968,8 +971,11 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>100406002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -985,8 +991,11 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>100406003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -1002,8 +1011,11 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>100406004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1019,8 +1031,11 @@
       <c r="E6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>100406005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -1036,8 +1051,11 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>100406009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -1053,8 +1071,11 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>100406010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -1070,8 +1091,11 @@
       <c r="E9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>100406011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -1087,8 +1111,11 @@
       <c r="E10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>100406012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>147</v>
       </c>
@@ -1104,8 +1131,11 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>100406013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -1121,8 +1151,11 @@
       <c r="E12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>100406014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -1138,8 +1171,11 @@
       <c r="E13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>100406015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>130</v>
       </c>
@@ -1155,8 +1191,11 @@
       <c r="E14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>100406020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>131</v>
       </c>
@@ -1172,8 +1211,11 @@
       <c r="E15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>100406026</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1189,8 +1231,11 @@
       <c r="E16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>100406027</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>132</v>
       </c>
@@ -1206,8 +1251,11 @@
       <c r="E17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>100406028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -1223,8 +1271,11 @@
       <c r="E18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>100406029</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>152</v>
       </c>
@@ -1240,8 +1291,11 @@
       <c r="E19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>100406030</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -1257,8 +1311,11 @@
       <c r="E20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>100406031</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>154</v>
       </c>
@@ -1274,8 +1331,11 @@
       <c r="E21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>100406032</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -1291,8 +1351,11 @@
       <c r="E22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>100406033</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>155</v>
       </c>
@@ -1308,8 +1371,11 @@
       <c r="E23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>100406034</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -1325,8 +1391,11 @@
       <c r="E24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>100406035</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -1342,8 +1411,11 @@
       <c r="E25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>100406036</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -1358,6 +1430,9 @@
       </c>
       <c r="E26" t="s">
         <v>21</v>
+      </c>
+      <c r="F26">
+        <v>100406100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>